<commit_message>
Fixed some minor bugs and added data from excel spreadsheet
</commit_message>
<xml_diff>
--- a/database_sisters/justPlayin/3.xlsx
+++ b/database_sisters/justPlayin/3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bridg\PycharmProjects\database-sisters\database_sisters\justPlayin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlucktong/Documents/GitHub/database-sisters/database_sisters/justPlayin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D964464-D4D0-4FF7-ACE3-C7B87CB1B40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC34C2E4-FC62-5546-938F-EF7ED3F9BD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9270" yWindow="0" windowWidth="11250" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="736">
   <si>
     <t>1786-09-04</t>
   </si>
@@ -12920,13 +12920,16 @@
   <si>
     <t>https://drive.google.com/file/d/14EIiAlvZR522cctNpw4XhE0ojasPVvG1/view?usp=drive_link</t>
   </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -12971,7 +12974,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -13282,22 +13285,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C122" workbookViewId="0">
-      <selection activeCell="D223" sqref="D223"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="78.9296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.19921875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.73046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="79" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="5.59765625" style="1"/>
+    <col min="7" max="16384" width="5.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13317,7 +13320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -13337,7 +13340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -13354,7 +13357,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -13374,7 +13377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -13394,7 +13397,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -13411,7 +13414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -13425,7 +13428,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -13442,7 +13445,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -13459,7 +13462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -13476,7 +13479,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -13493,7 +13496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -13507,7 +13510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -13524,7 +13527,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -13538,7 +13541,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
@@ -13555,7 +13558,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -13572,7 +13575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -13586,7 +13589,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
@@ -13603,7 +13606,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>69</v>
       </c>
@@ -13620,7 +13623,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>72</v>
       </c>
@@ -13637,7 +13640,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -13654,7 +13657,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -13674,7 +13677,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>83</v>
       </c>
@@ -13691,7 +13694,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>86</v>
       </c>
@@ -13705,7 +13708,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
@@ -13722,7 +13725,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>93</v>
       </c>
@@ -13739,7 +13742,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
@@ -13753,7 +13756,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>97</v>
       </c>
@@ -13767,7 +13770,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>102</v>
       </c>
@@ -13781,7 +13784,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>105</v>
       </c>
@@ -13798,7 +13801,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>108</v>
       </c>
@@ -13815,7 +13818,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -13829,7 +13832,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>108</v>
       </c>
@@ -13846,7 +13849,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>108</v>
       </c>
@@ -13860,7 +13863,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>116</v>
       </c>
@@ -13877,7 +13880,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>116</v>
       </c>
@@ -13891,7 +13894,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>116</v>
       </c>
@@ -13908,7 +13911,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>121</v>
       </c>
@@ -13925,7 +13928,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>121</v>
       </c>
@@ -13942,7 +13945,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>126</v>
       </c>
@@ -13956,7 +13959,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>126</v>
       </c>
@@ -13973,7 +13976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>126</v>
       </c>
@@ -13987,7 +13990,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>126</v>
       </c>
@@ -14001,7 +14004,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>126</v>
       </c>
@@ -14018,7 +14021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>137</v>
       </c>
@@ -14032,7 +14035,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>137</v>
       </c>
@@ -14049,7 +14052,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>137</v>
       </c>
@@ -14066,7 +14069,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>137</v>
       </c>
@@ -14080,7 +14083,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>137</v>
       </c>
@@ -14094,7 +14097,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
@@ -14111,7 +14114,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>147</v>
       </c>
@@ -14128,7 +14131,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>151</v>
       </c>
@@ -14145,7 +14148,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>155</v>
       </c>
@@ -14162,7 +14165,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>158</v>
       </c>
@@ -14179,7 +14182,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>161</v>
       </c>
@@ -14193,7 +14196,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>165</v>
       </c>
@@ -14203,8 +14206,11 @@
       <c r="C56" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F56" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>165</v>
       </c>
@@ -14221,7 +14227,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>170</v>
       </c>
@@ -14238,7 +14244,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>175</v>
       </c>
@@ -14255,7 +14261,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>179</v>
       </c>
@@ -14272,7 +14278,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>183</v>
       </c>
@@ -14286,7 +14292,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>186</v>
       </c>
@@ -14300,7 +14306,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>190</v>
       </c>
@@ -14314,7 +14320,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>194</v>
       </c>
@@ -14334,7 +14340,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>199</v>
       </c>
@@ -14351,7 +14357,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>204</v>
       </c>
@@ -14368,7 +14374,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>208</v>
       </c>
@@ -14388,7 +14394,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>213</v>
       </c>
@@ -14405,7 +14411,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>217</v>
       </c>
@@ -14422,7 +14428,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>217</v>
       </c>
@@ -14436,7 +14442,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>217</v>
       </c>
@@ -14450,7 +14456,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>217</v>
       </c>
@@ -14467,7 +14473,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>217</v>
       </c>
@@ -14481,7 +14487,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>230</v>
       </c>
@@ -14495,7 +14501,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>233</v>
       </c>
@@ -14509,7 +14515,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>236</v>
       </c>
@@ -14529,7 +14535,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>240</v>
       </c>
@@ -14543,7 +14549,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>243</v>
       </c>
@@ -14563,7 +14569,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>247</v>
       </c>
@@ -14577,7 +14583,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>247</v>
       </c>
@@ -14591,7 +14597,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>247</v>
       </c>
@@ -14608,7 +14614,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>255</v>
       </c>
@@ -14622,7 +14628,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>257</v>
       </c>
@@ -14639,7 +14645,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>261</v>
       </c>
@@ -14656,7 +14662,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>265</v>
       </c>
@@ -14670,7 +14676,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>268</v>
       </c>
@@ -14684,7 +14690,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>268</v>
       </c>
@@ -14698,7 +14704,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>273</v>
       </c>
@@ -14718,7 +14724,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>273</v>
       </c>
@@ -14732,7 +14738,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>279</v>
       </c>
@@ -14749,7 +14755,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>283</v>
       </c>
@@ -14763,7 +14769,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>285</v>
       </c>
@@ -14777,7 +14783,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>287</v>
       </c>
@@ -14797,7 +14803,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>291</v>
       </c>
@@ -14814,7 +14820,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>295</v>
       </c>
@@ -14828,7 +14834,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>298</v>
       </c>
@@ -14845,7 +14851,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>298</v>
       </c>
@@ -14859,7 +14865,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>298</v>
       </c>
@@ -14873,7 +14879,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>306</v>
       </c>
@@ -14890,7 +14896,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>310</v>
       </c>
@@ -14907,7 +14913,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>310</v>
       </c>
@@ -14924,7 +14930,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>317</v>
       </c>
@@ -14938,7 +14944,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>320</v>
       </c>
@@ -14952,7 +14958,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>320</v>
       </c>
@@ -14966,7 +14972,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>324</v>
       </c>
@@ -14983,7 +14989,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>328</v>
       </c>
@@ -14997,7 +15003,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>328</v>
       </c>
@@ -15014,7 +15020,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>334</v>
       </c>
@@ -15031,7 +15037,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>337</v>
       </c>
@@ -15045,7 +15051,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>340</v>
       </c>
@@ -15062,7 +15068,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>340</v>
       </c>
@@ -15076,7 +15082,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>346</v>
       </c>
@@ -15093,7 +15099,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>346</v>
       </c>
@@ -15110,7 +15116,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>352</v>
       </c>
@@ -15127,7 +15133,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>356</v>
       </c>
@@ -15141,7 +15147,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>359</v>
       </c>
@@ -15155,7 +15161,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>362</v>
       </c>
@@ -15169,7 +15175,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>365</v>
       </c>
@@ -15186,7 +15192,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>369</v>
       </c>
@@ -15203,7 +15209,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>369</v>
       </c>
@@ -15220,7 +15226,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>375</v>
       </c>
@@ -15234,7 +15240,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>378</v>
       </c>
@@ -15251,7 +15257,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>378</v>
       </c>
@@ -15268,7 +15274,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>383</v>
       </c>
@@ -15288,7 +15294,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>388</v>
       </c>
@@ -15302,7 +15308,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>392</v>
       </c>
@@ -15322,7 +15328,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>397</v>
       </c>
@@ -15336,7 +15342,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>401</v>
       </c>
@@ -15353,7 +15359,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>405</v>
       </c>
@@ -15370,7 +15376,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>408</v>
       </c>
@@ -15387,7 +15393,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>412</v>
       </c>
@@ -15404,7 +15410,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>415</v>
       </c>
@@ -15421,7 +15427,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>419</v>
       </c>
@@ -15435,7 +15441,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>422</v>
       </c>
@@ -15452,7 +15458,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>419</v>
       </c>
@@ -15469,7 +15475,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>419</v>
       </c>
@@ -15483,7 +15489,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>430</v>
       </c>
@@ -15500,7 +15506,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>434</v>
       </c>
@@ -15517,7 +15523,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>438</v>
       </c>
@@ -15531,7 +15537,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>441</v>
       </c>
@@ -15545,7 +15551,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>444</v>
       </c>
@@ -15562,7 +15568,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>448</v>
       </c>
@@ -15579,7 +15585,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>452</v>
       </c>
@@ -15593,7 +15599,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>456</v>
       </c>
@@ -15610,7 +15616,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>460</v>
       </c>
@@ -15627,7 +15633,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>460</v>
       </c>
@@ -15641,7 +15647,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>465</v>
       </c>
@@ -15658,7 +15664,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>469</v>
       </c>
@@ -15675,7 +15681,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>473</v>
       </c>
@@ -15689,7 +15695,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>473</v>
       </c>
@@ -15703,7 +15709,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>478</v>
       </c>
@@ -15717,7 +15723,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>481</v>
       </c>
@@ -15734,7 +15740,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>481</v>
       </c>
@@ -15748,7 +15754,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>487</v>
       </c>
@@ -15768,7 +15774,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>491</v>
       </c>
@@ -15785,7 +15791,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>491</v>
       </c>
@@ -15799,7 +15805,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>496</v>
       </c>
@@ -15816,7 +15822,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>500</v>
       </c>
@@ -15830,7 +15836,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>503</v>
       </c>
@@ -15844,7 +15850,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>503</v>
       </c>
@@ -15858,7 +15864,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>509</v>
       </c>
@@ -15875,7 +15881,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>514</v>
       </c>
@@ -15889,7 +15895,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>517</v>
       </c>
@@ -15906,7 +15912,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>520</v>
       </c>
@@ -15920,7 +15926,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>520</v>
       </c>
@@ -15937,7 +15943,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>527</v>
       </c>
@@ -15951,7 +15957,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>527</v>
       </c>
@@ -15968,7 +15974,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>533</v>
       </c>
@@ -15988,7 +15994,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>536</v>
       </c>
@@ -16008,7 +16014,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>540</v>
       </c>
@@ -16025,7 +16031,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>543</v>
       </c>
@@ -16042,7 +16048,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>546</v>
       </c>
@@ -16059,7 +16065,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>550</v>
       </c>
@@ -16073,7 +16079,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>553</v>
       </c>
@@ -16090,7 +16096,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>556</v>
       </c>
@@ -16104,7 +16110,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>559</v>
       </c>
@@ -16121,7 +16127,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>559</v>
       </c>
@@ -16135,7 +16141,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>559</v>
       </c>
@@ -16152,7 +16158,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>567</v>
       </c>
@@ -16163,7 +16169,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>569</v>
       </c>
@@ -16177,7 +16183,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>572</v>
       </c>
@@ -16191,7 +16197,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>574</v>
       </c>
@@ -16208,7 +16214,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>578</v>
       </c>
@@ -16222,7 +16228,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>581</v>
       </c>
@@ -16236,7 +16242,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>567</v>
       </c>
@@ -16253,7 +16259,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>588</v>
       </c>
@@ -16270,7 +16276,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>592</v>
       </c>
@@ -16284,7 +16290,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>596</v>
       </c>
@@ -16301,7 +16307,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>601</v>
       </c>
@@ -16318,7 +16324,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>605</v>
       </c>
@@ -16332,7 +16338,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>609</v>
       </c>
@@ -16349,7 +16355,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>613</v>
       </c>
@@ -16366,7 +16372,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>616</v>
       </c>
@@ -16383,7 +16389,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>620</v>
       </c>
@@ -16397,7 +16403,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>623</v>
       </c>
@@ -16414,7 +16420,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>623</v>
       </c>
@@ -16431,7 +16437,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>623</v>
       </c>
@@ -16445,7 +16451,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>633</v>
       </c>
@@ -16459,7 +16465,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>637</v>
       </c>
@@ -16479,7 +16485,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>637</v>
       </c>
@@ -16490,7 +16496,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>641</v>
       </c>
@@ -16507,7 +16513,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>645</v>
       </c>
@@ -16524,7 +16530,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>650</v>
       </c>
@@ -16541,7 +16547,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>654</v>
       </c>
@@ -16558,7 +16564,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>657</v>
       </c>
@@ -16572,7 +16578,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
         <v>660</v>
       </c>
@@ -16589,7 +16595,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>664</v>
       </c>
@@ -16606,7 +16612,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>668</v>
       </c>
@@ -16626,7 +16632,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>668</v>
       </c>
@@ -16640,7 +16646,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>675</v>
       </c>
@@ -16657,7 +16663,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>679</v>
       </c>
@@ -16671,7 +16677,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>681</v>
       </c>
@@ -16688,7 +16694,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>685</v>
       </c>
@@ -16705,7 +16711,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>688</v>
       </c>
@@ -16722,7 +16728,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>692</v>
       </c>
@@ -16742,7 +16748,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
         <v>697</v>
       </c>

</xml_diff>